<commit_message>
added counties and plot
</commit_message>
<xml_diff>
--- a/lakedata_observation_tables.xlsx
+++ b/lakedata_observation_tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Camille\Desktop\Fishscapes\hsSurvey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003AFF66-E528-4F30-862C-0958649B4DC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D27F244-1D82-4AE0-8286-0F724385F2D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C9336A81-3E79-4B07-9E1C-C823DEACB63E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
   <si>
     <t>Lake-year observations for creel and ef DNR data</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Lake year observations with lake info</t>
+  </si>
+  <si>
+    <t>Counties</t>
   </si>
 </sst>
 </file>
@@ -140,11 +143,11 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55DE9044-4566-40E9-B6ED-FA7E8C1E4965}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,53 +474,56 @@
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="4"/>
       <c r="C1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>398</v>
       </c>
       <c r="C2">
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>245</v>
       </c>
       <c r="C3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>310</v>
+      </c>
+      <c r="C4">
         <v>201</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3">
-        <v>310</v>
-      </c>
-      <c r="C4">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <f>SUM(B2:B4)</f>
         <v>953</v>
       </c>
@@ -528,162 +534,171 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
       <c r="B6" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="4"/>
       <c r="C8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>94</v>
       </c>
       <c r="C9">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>103</v>
       </c>
       <c r="C10">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>44</v>
       </c>
       <c r="C11">
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <f>SUM(B9:B11)</f>
         <v>241</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="4"/>
       <c r="C14" t="s">
         <v>8</v>
       </c>
-      <c r="E14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="G14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>23</v>
       </c>
       <c r="C15">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="2">
         <v>12</v>
       </c>
       <c r="C16">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="2">
         <v>27</v>
       </c>
       <c r="C17">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="2">
         <f>SUM(B15:B17)</f>
         <v>62</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" s="4"/>
       <c r="C20" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="G20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="2">
         <v>390</v>
       </c>
       <c r="C21">
         <v>152</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="2">
         <v>243</v>
       </c>
       <c r="C22">
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="2">
         <v>302</v>
       </c>
       <c r="C23">
         <v>201</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="2">
         <f>SUM(B21:B23)</f>
         <v>935</v>
       </c>

</xml_diff>

<commit_message>
brining in NTL data and model it
</commit_message>
<xml_diff>
--- a/lakedata_observation_tables.xlsx
+++ b/lakedata_observation_tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Camille\Desktop\Fishscapes\hsSurvey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49BACC7-8AFB-42AC-A2D0-5803999CB4F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A84E409B-FC2F-4EC1-9803-1BC2F22797CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C9336A81-3E79-4B07-9E1C-C823DEACB63E}"/>
   </bookViews>
@@ -166,11 +166,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -488,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55DE9044-4566-40E9-B6ED-FA7E8C1E4965}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,10 +499,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
+      <c r="B1" s="5"/>
       <c r="C1" t="s">
         <v>8</v>
       </c>
@@ -523,7 +523,7 @@
       <c r="C2">
         <v>152</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>19</v>
       </c>
       <c r="H2" t="s">
@@ -543,7 +543,7 @@
       <c r="C3">
         <v>77</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -557,7 +557,7 @@
       <c r="C4">
         <v>201</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>21</v>
       </c>
     </row>
@@ -581,10 +581,10 @@
       <c r="B6" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="5"/>
       <c r="C8" t="s">
         <v>8</v>
       </c>
@@ -638,10 +638,10 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="4"/>
+      <c r="B14" s="5"/>
       <c r="C14" t="s">
         <v>8</v>
       </c>
@@ -695,10 +695,10 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="4"/>
+      <c r="B20" s="5"/>
       <c r="C20" t="s">
         <v>8</v>
       </c>
@@ -718,6 +718,11 @@
       </c>
       <c r="C21">
         <v>152</v>
+      </c>
+      <c r="G21" t="str">
+        <f>$G$2</f>
+        <v xml:space="preserve"> "FOREST"  "LANGLADE" "OCONTO"   "FLORENCE" "ONEIDA"   "VILAS"    "MARATHON" "LINCOLN"  "BARRON"   "WASHBURN" "SAWYER"  
+ "CHIPPEWA" "PRICE"    "IRON"     "RUSK"     "BURNETT"  "POLK"     "DOUGLAS"  "BAYFIELD" "ASHLAND" </v>
       </c>
       <c r="H21" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
subsets for ntl years +
</commit_message>
<xml_diff>
--- a/lakedata_observation_tables.xlsx
+++ b/lakedata_observation_tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Camille\Desktop\Fishscapes\hsSurvey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D9926F-4152-4ADB-AFEC-F6B5A70CE2F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C74D57-D095-41FB-B3D0-97D33A64826B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{C9336A81-3E79-4B07-9E1C-C823DEACB63E}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="72">
   <si>
     <t>Lake-year observations for creel and ef DNR data</t>
   </si>
@@ -163,15 +163,6 @@
     <t>ASHLAND</t>
   </si>
   <si>
-    <t>Bass Cty</t>
-  </si>
-  <si>
-    <t>Pan Cty</t>
-  </si>
-  <si>
-    <t>Wall Cty</t>
-  </si>
-  <si>
     <t>EAU CLAIRE</t>
   </si>
   <si>
@@ -184,9 +175,6 @@
     <t>N=</t>
   </si>
   <si>
-    <t>Bass=Wall Cty</t>
-  </si>
-  <si>
     <t>GeoDataWI</t>
   </si>
   <si>
@@ -245,6 +233,24 @@
   </si>
   <si>
     <t>2013-2018</t>
+  </si>
+  <si>
+    <t>Bass dataset</t>
+  </si>
+  <si>
+    <t>Wall dataset</t>
+  </si>
+  <si>
+    <t>Panfish dataset</t>
+  </si>
+  <si>
+    <t>Bass=Wall counties</t>
+  </si>
+  <si>
+    <t>*only county different of other datasets</t>
+  </si>
+  <si>
+    <t>GeoDataWI for HsSurvey fish data</t>
   </si>
 </sst>
 </file>
@@ -276,7 +282,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -310,11 +316,69 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -327,6 +391,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -643,7 +724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55DE9044-4566-40E9-B6ED-FA7E8C1E4965}">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -945,28 +1026,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F31C860E-96E7-4127-BDD1-6E08558CC556}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3">
+        <v>45</v>
+      </c>
+      <c r="C3">
         <v>20</v>
       </c>
       <c r="D3">
@@ -976,354 +1059,401 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C5" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="11">
+        <v>2018</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="F6" s="9"/>
+      <c r="H6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" s="6" t="s">
+      <c r="I11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6" t="s">
+      <c r="F12" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="E13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="9">
+        <v>2015</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F5">
-        <v>2018</v>
-      </c>
-      <c r="H5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="F14" s="9">
+        <v>2017</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="9"/>
+      <c r="H16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="9">
+        <v>2014</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="9">
+        <v>2010</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="H7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="H20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+    </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21" s="9"/>
+      <c r="H21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+    </row>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F22" s="9"/>
+      <c r="H22" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" t="s">
-        <v>56</v>
-      </c>
-      <c r="H9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10" t="s">
-        <v>57</v>
-      </c>
-      <c r="H10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" t="s">
-        <v>54</v>
-      </c>
-      <c r="F11" t="s">
-        <v>58</v>
-      </c>
-      <c r="H11" t="s">
-        <v>45</v>
-      </c>
-      <c r="I11" t="s">
-        <v>51</v>
-      </c>
-      <c r="J11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F12" t="s">
-        <v>59</v>
-      </c>
-      <c r="H12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13">
-        <v>2015</v>
-      </c>
-      <c r="H13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" t="s">
-        <v>55</v>
-      </c>
-      <c r="F14">
-        <v>2017</v>
-      </c>
-      <c r="H14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="F23" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" t="s">
-        <v>53</v>
-      </c>
-      <c r="H16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E17" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17">
-        <v>2014</v>
-      </c>
-      <c r="H17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" t="s">
-        <v>51</v>
-      </c>
-      <c r="F18">
-        <v>2010</v>
-      </c>
-      <c r="H18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" t="s">
-        <v>38</v>
-      </c>
-      <c r="E19" t="s">
-        <v>54</v>
-      </c>
-      <c r="F19" t="s">
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C24" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F24" s="9" t="s">
         <v>63</v>
-      </c>
-      <c r="H19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" t="s">
-        <v>54</v>
-      </c>
-      <c r="F20" t="s">
-        <v>64</v>
-      </c>
-      <c r="H20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" t="s">
-        <v>53</v>
-      </c>
-      <c r="H21" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22" t="s">
-        <v>53</v>
-      </c>
-      <c r="H22" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" t="s">
-        <v>27</v>
-      </c>
-      <c r="E23" t="s">
-        <v>65</v>
-      </c>
-      <c r="F23" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>31</v>
-      </c>
-      <c r="D24" t="s">
-        <v>31</v>
-      </c>
-      <c r="E24" t="s">
-        <v>68</v>
-      </c>
-      <c r="F24" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>